<commit_message>
added excel utility files
</commit_message>
<xml_diff>
--- a/LearningFramework/src/test/resources/data.xlsx
+++ b/LearningFramework/src/test/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Learning\LearningFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA24B753-E364-4F20-BD78-0FE3F183E4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2959AB2B-8299-4CAF-8ABE-970CB5A75842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{182F8FD8-576B-492B-82F3-8AD677CA1665}"/>
   </bookViews>
@@ -47,18 +47,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>kalesh220</t>
-  </si>
-  <si>
-    <t>swathi220</t>
-  </si>
-  <si>
-    <t>teja220</t>
-  </si>
-  <si>
-    <t>padma220</t>
-  </si>
-  <si>
     <t>kalesh@123</t>
   </si>
   <si>
@@ -69,6 +57,18 @@
   </si>
   <si>
     <t>padma@123</t>
+  </si>
+  <si>
+    <t>kalesh220@gmail.com</t>
+  </si>
+  <si>
+    <t>pavan220@gmail.com</t>
+  </si>
+  <si>
+    <t>teja220@gmail.com</t>
+  </si>
+  <si>
+    <t>padmasri220@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -454,12 +454,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -472,35 +472,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -509,6 +509,10 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{BB43E776-E12A-46CA-85F3-EF3BF9E35203}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{139FA1BE-9B7D-4D7D-98D5-A210172A197D}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{3500D53A-8C85-46DD-92F0-B414824B4DC4}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{7BF80428-EFA9-47D0-A776-9D0DC6ECBDC5}"/>
+    <hyperlink ref="A3" r:id="rId6" xr:uid="{B3087F97-5E22-4F7A-BF0E-8FAA4B0F3A80}"/>
+    <hyperlink ref="A4" r:id="rId7" xr:uid="{DC4D7AC6-D082-4FD0-88DD-2D68C0B0685D}"/>
+    <hyperlink ref="A5" r:id="rId8" xr:uid="{3D49E56F-1C5C-478D-8092-8DB3102D8A5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>